<commit_message>
Alterações no click criterio
</commit_message>
<xml_diff>
--- a/POCSenado01/ExcelSaida.xlsx
+++ b/POCSenado01/ExcelSaida.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442AFF4E-68DA-4EEC-837E-98D4175CC1E6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,11 +20,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Endereço de e-mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Identificador
+</t>
+  </si>
+  <si>
+    <t>lutisto@gmail.com</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,21 +350,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B624A6-C26C-4EDE-B0C7-4F9BD8B90875}">
-  <dimension ref="B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
+    <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>50066528</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -361,12 +385,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>